<commit_message>
Version 2.1.0.0 some bugs fixed
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Release/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Release/Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\bin\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81752B82-BBDA-4598-83F5-15FA647E1F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9004929-A9EF-4245-AAE0-181BBA0ADED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Fecha:</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>ESTADO</t>
+  </si>
+  <si>
+    <t>UBICACIÓN</t>
   </si>
 </sst>
 </file>
@@ -322,10 +325,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AY9"/>
+  <dimension ref="A2:AZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AV13" sqref="AV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,25 +718,26 @@
     <col min="48" max="48" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="51" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="16384" width="8.88671875" style="1"/>
+    <col min="52" max="52" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="L2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="F3" s="10" t="s">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="F3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
-    <row r="8" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -887,8 +891,11 @@
       <c r="AY8" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="AZ8" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>